<commit_message>
Udpate excel spreadsheet with SSOut slope/interecept corrections
</commit_message>
<xml_diff>
--- a/SSOut_DAC_ADC.xlsx
+++ b/SSOut_DAC_ADC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27706"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu-my.sharepoint.com/personal/calderon-madera_1_buckeyemail_osu_edu/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/calderon-madera.1/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94E75D66-B4F2-4AE7-94CA-B7134C8004DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{36A84654-797E-1846-9F96-0405145DCB95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{48FDCF66-476C-6546-B385-CAB6E0509C92}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{48FDCF66-476C-6546-B385-CAB6E0509C92}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -99,7 +99,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -118,6 +118,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Rockwell"/>
+      <family val="1"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -428,12 +429,12 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -468,7 +469,7 @@
         <v>4095</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -503,7 +504,7 @@
         <v>4095</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -538,7 +539,7 @@
         <v>4095</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -573,7 +574,7 @@
         <v>4095</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -608,7 +609,7 @@
         <v>4095</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -643,7 +644,7 @@
         <v>4095</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -678,7 +679,7 @@
         <v>4095</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -713,7 +714,7 @@
         <v>4095</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -748,7 +749,7 @@
         <v>4095</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -783,7 +784,7 @@
         <v>4095</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -818,7 +819,7 @@
         <v>4095</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -853,7 +854,7 @@
         <v>4095</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -888,7 +889,7 @@
         <v>4095</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -923,7 +924,7 @@
         <v>4095</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -958,7 +959,7 @@
         <v>4095</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -993,7 +994,7 @@
         <v>4095</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
@@ -1028,7 +1029,7 @@
         <v>4095</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -1063,7 +1064,7 @@
         <v>4095</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>

</xml_diff>